<commit_message>
Changed template.xlsx to create time slot bug
</commit_message>
<xml_diff>
--- a/src/template.xlsx
+++ b/src/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khs\Proton Drive\kristoferhelgi\My files\Code\Py\RVK_Borg_HmH\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://reykjavik-my.sharepoint.com/personal/hanna_kristin_sigurdardottir_reykjavik_is/Documents/Desktop/Barðastaðir RVK_HmH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522108B3-5F9B-40A3-992F-CB39C96C9B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{2EAB2053-0638-45B5-B12D-3AD7F3432F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F70BB7DA-1E26-4240-BC41-475FE8209699}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
   <si>
     <t>mán</t>
   </si>
@@ -33,6 +33,9 @@
     <t>þri</t>
   </si>
   <si>
+    <t>mið</t>
+  </si>
+  <si>
     <t>fim</t>
   </si>
   <si>
@@ -87,14 +90,35 @@
     <t>-</t>
   </si>
   <si>
-    <t>mið</t>
+    <t>16:00-21:00</t>
+  </si>
+  <si>
+    <t>23:00-09:00</t>
+  </si>
+  <si>
+    <t>08:00-15:00</t>
+  </si>
+  <si>
+    <t>10:00-22:00</t>
+  </si>
+  <si>
+    <t>15:00-22:00</t>
+  </si>
+  <si>
+    <t>08:01-15:31</t>
+  </si>
+  <si>
+    <t>08:01-16:01</t>
+  </si>
+  <si>
+    <t>15:31-22:01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +129,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -131,12 +163,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Venjulegt" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,44 +447,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -460,25 +493,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -488,15 +521,15 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -504,65 +537,65 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
+    <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -573,79 +606,78 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
+    <row r="10" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+    <row r="11" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+    <row r="14" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -653,15 +685,15 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -669,15 +701,15 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -685,139 +717,287 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>